<commit_message>
added sir sam's recommendation - make the bot speak when activated with wakeword
</commit_message>
<xml_diff>
--- a/chatbotdata.xlsx
+++ b/chatbotdata.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -470,7 +470,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2023-06-11 18:10:20</t>
+          <t>2023-06-20 20:50:27</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -480,243 +480,27 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>where is the room 803</t>
+          <t>hello</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>it is located at the 4th floor</t>
+          <t>Hello, my fantastic friend! How can I make your day shine even brighter?</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>LOC fourth floor location</t>
+          <t>GEN hello</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>3.562999999994645</v>
+        <v>2.782000000006519</v>
       </c>
       <c r="G2" t="n">
-        <v>9.671000000002095</v>
+        <v>17.5</v>
       </c>
       <c r="H2" t="n">
-        <v>13.23399999999674</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2023-06-11 18:11:10</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>hello ram</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>where is the room</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>it is located at the 7th floor</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>LOC seventh floor location</t>
-        </is>
-      </c>
-      <c r="F3" t="n">
-        <v>2.985000000000582</v>
-      </c>
-      <c r="G3" t="n">
-        <v>5.687000000005355</v>
-      </c>
-      <c r="H3" t="n">
-        <v>8.672000000005937</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2023-06-11 18:11:20</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>hello robi</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>where is the room</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>it is located at the 7th floor</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>LOC seventh floor location</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
-        <v>3.157000000006519</v>
-      </c>
-      <c r="G4" t="n">
-        <v>6.937000000005355</v>
-      </c>
-      <c r="H4" t="n">
-        <v>10.09400000001187</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2023-06-11 18:11:38</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>hello rami</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>where is the room</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>it is located at the 7th floor</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>LOC seventh floor location</t>
-        </is>
-      </c>
-      <c r="F5" t="n">
-        <v>4.01600000000326</v>
-      </c>
-      <c r="G5" t="n">
-        <v>9.968999999997322</v>
-      </c>
-      <c r="H5" t="n">
-        <v>13.98500000000058</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>2023-06-11 18:11:58</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>hello rami</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>where is 803</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>it is located at the 8th floor</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>LOC eighth floor location</t>
-        </is>
-      </c>
-      <c r="F6" t="n">
-        <v>3.061999999990803</v>
-      </c>
-      <c r="G6" t="n">
-        <v>6.969000000011874</v>
-      </c>
-      <c r="H6" t="n">
-        <v>10.03100000000268</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2023-06-11 18:13:19</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>hello rami</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>where is the admissions office</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>it is located here at the 1st floor</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>LOC lobby floor location</t>
-        </is>
-      </c>
-      <c r="F7" t="n">
-        <v>3.844000000011874</v>
-      </c>
-      <c r="G7" t="n">
-        <v>7.515999999988708</v>
-      </c>
-      <c r="H7" t="n">
-        <v>11.36000000000058</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>2023-06-11 18:13:31</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>hello robi</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>what does the admissions office do</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>it is located here at the 1st floor</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>LOC lobby floor location</t>
-        </is>
-      </c>
-      <c r="F8" t="n">
-        <v>3.73399999999674</v>
-      </c>
-      <c r="G8" t="n">
-        <v>8.60899999999674</v>
-      </c>
-      <c r="H8" t="n">
-        <v>12.34299999999348</v>
+        <v>20.28200000000652</v>
       </c>
     </row>
   </sheetData>

</xml_diff>